<commit_message>
Update test cases for MCA
</commit_message>
<xml_diff>
--- a/temp_email_mca.xlsx
+++ b/temp_email_mca.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t>Email</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>yvr03582@nezid.com</t>
+  </si>
+  <si>
+    <t>csm82631@zslsz.com</t>
   </si>
 </sst>
 </file>
@@ -89,7 +92,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
@@ -145,6 +148,11 @@
         <v>10</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>